<commit_message>
JOYSTICK 0: 12er-Tastatur, defines mit JOYSTICKTASTExy anschlagstruct erweitert mit richtung
anschlagvonmotor:
- pfeiltastenrichtung neu: kontrolle für ausgabe
-   auskommentiert:   //if (!(anschlagstatus & (1 << (END_A0 + motor)))) // Bit ist noch nicht gesetzt
</commit_message>
<xml_diff>
--- a/tastatur 3x3.xlsx
+++ b/tastatur 3x3.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Slave_32/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Slave_32_SPI_Draw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{101D1941-809C-C446-8C61-B1EF39EDD07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037D6A2E-AB23-A447-9D63-68705DA482CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="1020" windowWidth="28240" windowHeight="17240" xr2:uid="{87DFF654-CCBA-8643-A045-2FD3564ECEDD}"/>
+    <workbookView xWindow="1220" yWindow="1020" windowWidth="28240" windowHeight="17240" activeTab="1" xr2:uid="{87DFF654-CCBA-8643-A045-2FD3564ECEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tastatur 3x4 MILL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -803,6 +804,743 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tastatur 3x4 MILL'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49F8-8C49-9679-1B187F686E53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tastatur 3x4 MILL'!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>185</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-49F8-8C49-9679-1B187F686E53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1516044048"/>
+        <c:axId val="1516061696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1516044048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1516061696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1516061696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1516044048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tastatur 3x4 MILL'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-12A8-3647-9DDB-1B86B014504A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tastatur 3x4 MILL'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-12A8-3647-9DDB-1B86B014504A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="265420128"/>
+        <c:axId val="266181568"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="265420128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266181568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="266181568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265420128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -883,6 +1621,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1387,6 +2205,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1950,6 +3774,87 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AA92B77-00F2-8A4A-845C-45C912C2E020}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{129D0DB0-E14A-8347-A320-C6956EC4C865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2265,7 +4170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E854E49E-F133-EC41-9712-7AC7FCD8BBC1}">
   <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -2419,4 +4324,272 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EF9CDF-35D3-A04E-B94E-D5F952882912}">
+  <dimension ref="A2:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <f>ROUND((B3+B2)/2,0)</f>
+        <v>17</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"#define KEY"&amp;A2&amp;"  "&amp;C2</f>
+        <v>#define KEY1  17</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"#define JOYSTICKTASTE"&amp;A2&amp;"  "&amp;C2</f>
+        <v>#define JOYSTICKTASTE1  17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">ROUND((B4+B3)/2,0)</f>
+        <v>27</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E13" si="1">"#define KEY"&amp;A3&amp;"  "&amp;C3</f>
+        <v>#define KEY2  27</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G13" si="2">"#define JOYSTICKTASTE"&amp;A3&amp;"  "&amp;C3</f>
+        <v>#define JOYSTICKTASTE2  27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY3  41</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE3  41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY4  63</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE4  63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY5  90</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE5  90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>103</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY6  120</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE6  120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>137</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY7  155</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE7  155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>173</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY8  185</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE8  185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>196</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>206</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY9  206</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE9  206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>216</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY10  224</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE10  224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>232</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>236</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY11  236</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE11  236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>240</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>#define KEY12  248</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#define JOYSTICKTASTE12  248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>